<commit_message>
fix techstates array; test
</commit_message>
<xml_diff>
--- a/dyson.xlsx
+++ b/dyson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnels\Documents\livesplit.autosplitter.dysonsphereprogram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0389FBB9-23C5-494F-BB61-959EAF11283B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1672B3C3-24F0-471E-B8CA-56967B9A7043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{1C2348D9-57B4-4B73-A089-83728E547E59}"/>
+    <workbookView xWindow="570" yWindow="4065" windowWidth="25905" windowHeight="11970" activeTab="1" xr2:uid="{1C2348D9-57B4-4B73-A089-83728E547E59}"/>
   </bookViews>
   <sheets>
     <sheet name="techState" sheetId="6" r:id="rId1"/>
@@ -1990,9 +1990,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2102,7 +2102,7 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2119,11 +2119,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8544,10 +8544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93A4BD1-7B9B-416E-97ED-15D629DA9614}">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8587,7 +8587,7 @@
         <v>611</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B69" si="1">1+B2</f>
+        <f t="shared" ref="B3:B68" si="1">1+B2</f>
         <v>3</v>
       </c>
       <c r="C3" t="str">
@@ -8903,7 +8903,7 @@
         <v>27</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" ref="C27:C91" si="2">_xlfn.CONCAT(B27,". ",A27)</f>
+        <f t="shared" ref="C27:C90" si="2">_xlfn.CONCAT(B27,". ",A27)</f>
         <v>27. Blue Science (6/s, 18x Labs)</v>
       </c>
     </row>
@@ -9157,1524 +9157,1515 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <f>1+B46</f>
+        <v>47</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="2"/>
+        <v>47. RS - +100 MW Power</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B48">
-        <f>1+B46</f>
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="2"/>
-        <v>47. RS - +100 MW Power</v>
+        <v>48. Energy Circuit 1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B49">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
-        <v>48. Energy Circuit 1</v>
+        <v>49. RS - Energetic Graphite (12/s)</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B50">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
-        <v>49. RS - Energetic Graphite (12/s)</v>
+        <v>50. RS - Oil Extractors (24/s)</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B51">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
-        <v>50. RS - Oil Extractors (24/s)</v>
+        <v>51. RS - Refineries (48x)</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B52">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
-        <v>51. RS - Refineries (48x)</v>
+        <v>52. RS - Hydrogen (12/s)</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B53">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
-        <v>52. RS - Hydrogen (12/s)</v>
+        <v>53. Red Science (6/s, 36 Labs)</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B54">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
-        <v>53. Red Science (6/s, 36 Labs)</v>
+        <v>54. Veins Utilization 1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B55">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="2"/>
-        <v>54. Veins Utilization 1</v>
+        <v>55. Drive Engine 2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
-        <v>55. Drive Engine 2</v>
+        <v>56. Drone Engine 2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B57">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="2"/>
-        <v>56. Drone Engine 2</v>
+        <v>57. Communication Control 2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B58">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
-        <v>57. Communication Control 2</v>
+        <v>58. Deuterium Fractionation</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B59">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
-        <v>58. Deuterium Fractionation</v>
+        <v>59. Mine Silicon</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="B60">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="2"/>
-        <v>59. Mine Silicon</v>
+        <v>60. Solar Panels</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>131</v>
+        <v>49</v>
       </c>
       <c r="B61">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="2"/>
-        <v>60. Solar Panels</v>
+        <v>61. Initial Deuterium Loop</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="B62">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
-        <v>61. Initial Deuterium Loop</v>
+        <v>62. Electric Motors</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B63">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
-        <v>62. Electric Motors</v>
+        <v>63. Sorter Mk II</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B64">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="2"/>
-        <v>63. Sorter Mk II</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>64. Water Pumps</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>134</v>
+        <v>52</v>
       </c>
       <c r="B65">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
-        <v>64. Water Pumps</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65. Communication Control 3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B66">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="2"/>
-        <v>65. Communication Control 3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66. Mecha Core 2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B67">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="2"/>
-        <v>66. Mecha Core 2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67. Inventory Capacity 2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="2"/>
-        <v>67. Inventory Capacity 2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>68. Titanium Smelting</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
-        <v>68</v>
+        <f t="shared" ref="B69:B132" si="3">1+B68</f>
+        <v>69</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="2"/>
-        <v>68. Titanium Smelting</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69. Mine Titanium</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B70">
-        <f t="shared" ref="B70:B133" si="3">1+B69</f>
-        <v>69</v>
+        <f t="shared" si="3"/>
+        <v>70</v>
       </c>
       <c r="C70" t="str">
-        <f t="shared" si="2"/>
-        <v>69. Mine Titanium</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT(B70,". ",A70)</f>
+        <v>70. High-Strength Titanium Alloy</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="C71" t="e">
-        <f>_xlfn.CONCAT(B71,". ",#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="2"/>
+        <v>71. Mechanical Frame 1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B72">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="2"/>
-        <v>71. Mechanical Frame 1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>72. Mechanical Frame 2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B73">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="2"/>
-        <v>72. Mechanical Frame 2</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73. Mechanical Frame 3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B74">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="2"/>
-        <v>73. Mechanical Frame 3</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74. High-efficiency Logistics System</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="B75">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="2"/>
-        <v>74. High-efficiency Logistics System</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75. Electromagnetic Turbine</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B76">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="2"/>
-        <v>75. Electromagnetic Turbine</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>76. Sorter Mk III</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C77" t="str">
-        <f t="shared" si="2"/>
-        <v>76. Sorter Mk III</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT(B77,". ",A77)</f>
+        <v>77. Basic Chemical Engineering</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C78" t="str">
-        <f>_xlfn.CONCAT(B78,". ",E73)</f>
-        <v>77. Basic Chemical Engineering</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>78. Polymer Chemical Engineering</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C79" t="str">
-        <f t="shared" si="2"/>
-        <v>78. Polymer Chemical Engineering</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <f>_xlfn.CONCAT(B79,". ",A79)</f>
+        <v>79. Applied Superconductor</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C80" t="str">
-        <f>_xlfn.CONCAT(B80,". ",E74)</f>
-        <v>79. Applied Superconductor</v>
+        <f t="shared" si="2"/>
+        <v>80. High-Strength Crystal</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="2"/>
-        <v>80. High-Strength Crystal</v>
+        <v>81. Structure Matrix</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="2"/>
-        <v>81. Structure Matrix</v>
+        <v>82. Chemical Plants</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="2"/>
-        <v>82. Chemical Plants</v>
+        <v>83. Sulfuric Acid</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="2"/>
-        <v>83. Sulfuric Acid</v>
+        <v>84. Graphene</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="2"/>
-        <v>84. Graphene</v>
+        <v>85. Particle Container</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="2"/>
-        <v>85. Particle Container</v>
+        <v>86. Microcrystalline Component</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="2"/>
-        <v>86. Microcrystalline Component</v>
+        <v>87. Processor</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="2"/>
-        <v>87. Processor</v>
+        <v>88. Planetary Logistics Stations</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="2"/>
-        <v>88. Planetary Logistics Stations</v>
+        <v>89. Thruster</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="2"/>
-        <v>89. Thruster</v>
+        <v>90. Logistics Drones</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>144</v>
+        <v>68</v>
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C91" t="str">
-        <f t="shared" si="2"/>
-        <v>90. Logistics Drones</v>
+        <f t="shared" ref="C91:C154" si="4">_xlfn.CONCAT(B91,". ",A91)</f>
+        <v>91. Limited Yellow Science (120)</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C92" t="str">
-        <f t="shared" ref="C92:C155" si="4">_xlfn.CONCAT(B92,". ",A92)</f>
-        <v>91. Limited Yellow Science (120)</v>
+        <f t="shared" si="4"/>
+        <v>92. Interstellar Logistics System</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="4"/>
-        <v>92. Interstellar Logistics System</v>
+        <v>93. Titanium Alloy (8 stacks)</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="4"/>
-        <v>93. Titanium Alloy (8 stacks)</v>
+        <v>94. Interplanetary Logistics Stations</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="4"/>
-        <v>94. Interplanetary Logistics Stations</v>
+        <v>95. Reinforce Thruster</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B96">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="4"/>
-        <v>95. Reinforce Thruster</v>
+        <v>96. Logistics Vessel</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>148</v>
+        <v>70</v>
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="4"/>
-        <v>96. Logistics Vessel</v>
+        <v>97. YS - +130 MW Power</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="4"/>
-        <v>97. YS - +130 MW Power</v>
+        <v>98. YS - Energitic Graphite (18/s)</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="4"/>
-        <v>98. YS - Energitic Graphite (18/s)</v>
+        <v>99. YS - Diamonds (6/s)</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="4"/>
-        <v>99. YS - Diamonds (6/s)</v>
+        <v>100. YS - Water (6/s)</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B101">
         <f t="shared" si="3"/>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="4"/>
-        <v>100. YS - Water (6/s)</v>
+        <v>101. YS - Oil Extractors (+6/s)</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B102">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="4"/>
-        <v>101. YS - Oil Extractors (+6/s)</v>
+        <v>102. YS - Oil Refineries (12x)</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B103">
         <f t="shared" si="3"/>
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="4"/>
-        <v>102. YS - Oil Refineries (12x)</v>
+        <v>103. YS - Plastic (12/s)</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B104">
         <f t="shared" si="3"/>
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="4"/>
-        <v>103. YS - Plastic (12/s)</v>
+        <v>104. YS - Organic Crystal (6/s)</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B105">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="4"/>
-        <v>104. YS - Organic Crystal (6/s)</v>
+        <v>105. YS - Titanium Crystal (6/s)</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B106">
         <f t="shared" si="3"/>
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="4"/>
-        <v>105. YS - Titanium Crystal (6/s)</v>
+        <v>106. Yellow Science (6/s, 48 Labs)</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B107">
         <f t="shared" si="3"/>
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="4"/>
-        <v>106. Yellow Science (6/s, 48 Labs)</v>
+        <v>107. Veins Utilization 2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B108">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="4"/>
-        <v>107. Veins Utilization 2</v>
+        <v>108. Gas Giant Exploitation</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="B109">
         <f t="shared" si="3"/>
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="4"/>
-        <v>108. Gas Giant Exploitation</v>
+        <v>109. Crystal Silicon</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="B110">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="4"/>
-        <v>109. Crystal Silicon</v>
+        <v>110. Super-magentic Ring</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B111">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="4"/>
-        <v>110. Super-magentic Ring</v>
+        <v>111. Accumulator</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="B112">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="4"/>
-        <v>111. Accumulator</v>
+        <v>112. Energy Exchanger</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="B113">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="4"/>
-        <v>112. Energy Exchanger</v>
+        <v>113. Orbital Collectors</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B114">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="4"/>
-        <v>113. Orbital Collectors</v>
+        <v>114. Belt Mk III</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="B115">
         <f t="shared" si="3"/>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="4"/>
-        <v>114. Belt Mk III</v>
+        <v>115. PS - +?MW Power</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B116">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="4"/>
-        <v>115. PS - +?MW Power</v>
+        <v>116. PS - Iron Ingots (24/s)</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B117">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="4"/>
-        <v>116. PS - Iron Ingots (24/s)</v>
+        <v>117. PS - Copper Ingots (48/s)</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B118">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="4"/>
-        <v>117. PS - Copper Ingots (48/s)</v>
+        <v>118. PS - HP Silicon Ingots (60/s)</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B119">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="4"/>
-        <v>118. PS - HP Silicon Ingots (60/s)</v>
+        <v>119. PS - Microcrystalline (24/s)</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B120">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="4"/>
-        <v>119. PS - Microcrystalline (24/s)</v>
+        <v>120. PS - Circuit Boards (24/s)</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B121">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="4"/>
-        <v>120. PS - Circuit Boards (24/s)</v>
+        <v>121. PS - Processors (12/s)</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B122">
         <f t="shared" si="3"/>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="4"/>
-        <v>121. PS - Processors (12/s)</v>
+        <v>122. PS - Energetic Graphite (6/s)</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B123">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="4"/>
-        <v>122. PS - Energetic Graphite (6/s)</v>
+        <v>123. PS - Oil Extractors (+6/s)</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B124">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="4"/>
-        <v>123. PS - Oil Extractors (+6/s)</v>
+        <v>124. PS - Oil Refineries (12x)</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B125">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="4"/>
-        <v>124. PS - Oil Refineries (12x)</v>
+        <v>125. PS - Titanium Ingot (6/s)</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B126">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="4"/>
-        <v>125. PS - Titanium Ingot (6/s)</v>
+        <v>126. PS - Fire Ice (18/s)</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B127">
         <f t="shared" si="3"/>
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="4"/>
-        <v>126. PS - Fire Ice (18/s)</v>
+        <v>127. PS - Graphene (Fire Ice) (18/s)</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B128">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="4"/>
-        <v>127. PS - Graphene (Fire Ice) (18/s)</v>
+        <v>128. PS - Nanotubes (12/s)</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B129">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="4"/>
-        <v>128. PS - Nanotubes (12/s)</v>
+        <v>129. PS - Crystal Silicon (12/s)</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B130">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="4"/>
-        <v>129. PS - Crystal Silicon (12/s)</v>
+        <v>130. PS - Particle Broadband (6/s)</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B131">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" si="4"/>
-        <v>130. PS - Particle Broadband (6/s)</v>
+        <v>131. Purple Science (6/s, 60 Labs)</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B132">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="4"/>
-        <v>131. Purple Science (6/s, 60 Labs)</v>
+        <v>132. Veins Utilization 3</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B133">
-        <f t="shared" si="3"/>
-        <v>132</v>
+        <f t="shared" ref="B133:B162" si="5">1+B132</f>
+        <v>133</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="4"/>
-        <v>132. Veins Utilization 3</v>
+        <v>133. Veins Utilization 4</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="B134">
-        <f t="shared" ref="B134:B163" si="5">1+B133</f>
-        <v>133</v>
+        <f t="shared" si="5"/>
+        <v>134</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="4"/>
-        <v>133. Veins Utilization 4</v>
+        <v>134. Fractionators (5 stacks)</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="B135">
         <f t="shared" si="5"/>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="4"/>
-        <v>134. Fractionators (5 stacks)</v>
+        <v>135. Universe Exploration 3</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B136">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="4"/>
-        <v>135. Universe Exploration 3</v>
+        <v>136. Build 2 Space Warpers</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B137">
         <f t="shared" si="5"/>
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="4"/>
-        <v>136. Build 2 Space Warpers</v>
+        <v>137. GS - +?MW Power</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B138">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="4"/>
-        <v>137. GS - +?MW Power</v>
+        <v>138. GS - Organic Crystal (6/s)</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B139">
         <f t="shared" si="5"/>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="4"/>
-        <v>138. GS - Organic Crystal (6/s)</v>
+        <v>139. GS - Energetic Graphite (12/s)</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B140">
         <f t="shared" si="5"/>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="4"/>
-        <v>139. GS - Energetic Graphite (12/s)</v>
+        <v>140. GS - Diamond (12/s)</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B141">
         <f t="shared" si="5"/>
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="4"/>
-        <v>140. GS - Diamond (12/s)</v>
+        <v>141. GS - Particle Container (6/s)</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="B142">
         <f t="shared" si="5"/>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="4"/>
-        <v>141. GS - Particle Container (6/s)</v>
+        <v>142. GS - Deuterium (30/s)</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="B143">
         <f t="shared" si="5"/>
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="4"/>
-        <v>142. GS - Deuterium (30/s)</v>
+        <v>143. GS - Strange Matter (3/s)</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B144">
         <f t="shared" si="5"/>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="4"/>
-        <v>143. GS - Strange Matter (3/s)</v>
+        <v>144. GS - Graviton Lens (3/s)</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B145">
         <f t="shared" si="5"/>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="4"/>
-        <v>144. GS - Graviton Lens (3/s)</v>
+        <v>145. GS - Casimir Crystal (6/s)</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B146">
         <f t="shared" si="5"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="4"/>
-        <v>145. GS - Casimir Crystal (6/s)</v>
+        <v>146. GS - Quantum Chip (3/s)</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B147">
         <f t="shared" si="5"/>
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="4"/>
-        <v>146. GS - Quantum Chip (3/s)</v>
+        <v>147. GS - Processor (6/s)</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B148">
         <f t="shared" si="5"/>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="4"/>
-        <v>147. GS - Processor (6/s)</v>
+        <v>148. GS - Plane Filter (6/s)</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B149">
         <f t="shared" si="5"/>
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="4"/>
-        <v>148. GS - Plane Filter (6/s)</v>
+        <v>149. GS - Titanium Glass (12/s)</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B150">
         <f t="shared" si="5"/>
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="4"/>
-        <v>149. GS - Titanium Glass (12/s)</v>
+        <v>150. Green Science (6/s, 144 Labs)</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="B151">
         <f t="shared" si="5"/>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="4"/>
-        <v>150. Green Science (6/s, 144 Labs)</v>
+        <v>151. Frame Material</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B152">
         <f t="shared" si="5"/>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="4"/>
-        <v>151. Frame Material</v>
+        <v>152. Mini Particle Colliders</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B153">
         <f t="shared" si="5"/>
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="4"/>
-        <v>152. Mini Particle Colliders</v>
+        <v>153. Photon Combiner</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="B154">
         <f t="shared" si="5"/>
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="4"/>
-        <v>153. Photon Combiner</v>
+        <v>154. Ray Receivers</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="B155">
         <f t="shared" si="5"/>
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C155" t="str">
-        <f t="shared" si="4"/>
-        <v>154. Ray Receivers</v>
+        <f t="shared" ref="C155:C162" si="6">_xlfn.CONCAT(B155,". ",A155)</f>
+        <v>155. EM-Rail Ejectors (108)</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="B156">
         <f t="shared" si="5"/>
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C156" t="str">
-        <f t="shared" ref="C156:C163" si="6">_xlfn.CONCAT(B156,". ",A156)</f>
-        <v>155. EM-Rail Ejectors (108)</v>
+        <f t="shared" si="6"/>
+        <v>156. WS - Solar Sails (36/s)</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B157">
         <f t="shared" si="5"/>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="6"/>
-        <v>156. WS - Solar Sails (36/s)</v>
+        <v>157. WS - Ray Receivers</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B158">
         <f t="shared" si="5"/>
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="6"/>
-        <v>157. WS - Ray Receivers</v>
+        <v>158. WS - +4.50GW Power</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B159">
         <f t="shared" si="5"/>
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="6"/>
-        <v>158. WS - +4.50GW Power</v>
+        <v>159. WS - Critical Photon (6/s)</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B160">
         <f t="shared" si="5"/>
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="6"/>
-        <v>159. WS - Critical Photon (6/s)</v>
+        <v>160. WS - Antimatter (6/s)</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B161">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="6"/>
-        <v>160. WS - Antimatter (6/s)</v>
+        <v>161. White Science (6/s)</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B162">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="6"/>
-        <v>161. White Science (6/s)</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B163">
-        <f t="shared" si="5"/>
-        <v>162</v>
-      </c>
-      <c r="C163" t="str">
-        <f t="shared" si="6"/>
         <v>162. Mission Complete</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164">
-        <f>1+B163</f>
-        <v>163</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="3"/>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16344,8 +16335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59094B6E-8E1D-427C-A28F-3773A981F8B5}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J28" sqref="E28:J35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>